<commit_message>
CV pantalla de reportes de ventas, pantala de recibos emitidos nuevos reportes
</commit_message>
<xml_diff>
--- a/FALEC-w1-core-web/WebContent/reportes/FALECPV-FacAnuladas.xlsx
+++ b/FALEC-w1-core-web/WebContent/reportes/FALECPV-FacAnuladas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/projects/gitrepositorio/FacturaElectronica-App/FALEC-w1-core-web/WebContent/reportes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{573E6189-DB63-FE48-8840-CBB9C1EDF361}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3B739DE-7EA6-1B4A-A1B0-48DD0382B548}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1520" yWindow="7580" windowWidth="35960" windowHeight="18240" xr2:uid="{E9788733-D204-D84A-A824-443E01B2DF94}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>% IVA</t>
   </si>
@@ -60,9 +60,6 @@
     <t>ESTADO</t>
   </si>
   <si>
-    <t>AUT S.R.I.</t>
-  </si>
-  <si>
     <t>SUBTOTAL</t>
   </si>
   <si>
@@ -73,15 +70,6 @@
   </si>
   <si>
     <t>TOTAL</t>
-  </si>
-  <si>
-    <t>PAGO</t>
-  </si>
-  <si>
-    <t>ENTREGA</t>
-  </si>
-  <si>
-    <t>CAMBIO</t>
   </si>
   <si>
     <t>CANTIDAD</t>
@@ -97,7 +85,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -112,13 +100,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -170,19 +151,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -502,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F32A76B9-2613-7147-BFF0-D21843D4C7F8}">
-  <dimension ref="A2:P10"/>
+  <dimension ref="A2:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -513,92 +491,81 @@
     <col min="1" max="1" width="17.83203125" customWidth="1"/>
     <col min="2" max="2" width="17.6640625" customWidth="1"/>
     <col min="3" max="3" width="31.6640625" customWidth="1"/>
-    <col min="4" max="6" width="22.5" customWidth="1"/>
-    <col min="7" max="8" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5" customWidth="1"/>
-    <col min="11" max="12" width="8.5" customWidth="1"/>
-    <col min="13" max="14" width="13.5" customWidth="1"/>
-    <col min="15" max="15" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.33203125" customWidth="1"/>
+    <col min="4" max="5" width="22.5" customWidth="1"/>
+    <col min="6" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5" customWidth="1"/>
+    <col min="10" max="11" width="8.5" customWidth="1"/>
+    <col min="12" max="12" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
+    <row r="2" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -615,42 +582,30 @@
         <v>10</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K10" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>0</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="N10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="P10" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A2:P2"/>
+    <mergeCell ref="A2:L2"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B8:D8"/>

</xml_diff>

<commit_message>
CV, refactorixación de fabricante, categroría, reporte de ventas se implementa para escoger establecimeinto, pantalla de panel se implementa para seleccionar establecieminto
</commit_message>
<xml_diff>
--- a/FALEC-w1-core-web/WebContent/reportes/FALECPV-FacAnuladas.xlsx
+++ b/FALEC-w1-core-web/WebContent/reportes/FALECPV-FacAnuladas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/projects/gitrepositorio/FacturaElectronica-App/FALEC-w1-core-web/WebContent/reportes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3B739DE-7EA6-1B4A-A1B0-48DD0382B548}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7DEE8BF-E579-654F-B53C-5E31107ECE2A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1520" yWindow="7580" windowWidth="35960" windowHeight="18240" xr2:uid="{E9788733-D204-D84A-A824-443E01B2DF94}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>% IVA</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>TOT SIN IVA</t>
+  </si>
+  <si>
+    <t>EMPRESA:</t>
+  </si>
+  <si>
+    <t>SUCURSAL</t>
   </si>
 </sst>
 </file>
@@ -480,26 +486,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F32A76B9-2613-7147-BFF0-D21843D4C7F8}">
-  <dimension ref="A2:L10"/>
+  <dimension ref="A2:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.83203125" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
-    <col min="3" max="3" width="31.6640625" customWidth="1"/>
-    <col min="4" max="5" width="22.5" customWidth="1"/>
-    <col min="6" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5" customWidth="1"/>
-    <col min="10" max="11" width="8.5" customWidth="1"/>
-    <col min="12" max="12" width="13.5" customWidth="1"/>
+    <col min="2" max="3" width="17.6640625" customWidth="1"/>
+    <col min="4" max="4" width="31.6640625" customWidth="1"/>
+    <col min="5" max="6" width="22.5" customWidth="1"/>
+    <col min="7" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5" customWidth="1"/>
+    <col min="11" max="12" width="8.5" customWidth="1"/>
+    <col min="13" max="13" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>16</v>
       </c>
@@ -514,103 +520,117 @@
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
-      <c r="E5" s="3"/>
+      <c r="E5" s="5"/>
       <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
-      <c r="E6" s="3"/>
+      <c r="E6" s="5"/>
       <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
-      <c r="E7" s="3"/>
+      <c r="E7" s="5"/>
       <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
-      <c r="E8" s="3"/>
+      <c r="E8" s="5"/>
       <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="K10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="L10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="M10" s="1" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A2:L2"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
+  <mergeCells count="7">
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="G4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>